<commit_message>
Updated with new boxes for blocks
</commit_message>
<xml_diff>
--- a/esc project template.xlsx
+++ b/esc project template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\todolist\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tjuny\Documents\School\Term 5\ESC\ReactJS\Demo\50.003-Frontend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E928CB-7CBA-4C3A-9224-8617B8D6FBF1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{903FDE07-099E-48D1-926B-47C61DF70DCF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{3C774843-307A-40CD-85CD-B70ACD0E23E3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{3C774843-307A-40CD-85CD-B70ACD0E23E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="59">
   <si>
     <t>Project Name</t>
   </si>
@@ -63,73 +63,151 @@
     <t>Engineer</t>
   </si>
   <si>
-    <t>happy123 project</t>
-  </si>
-  <si>
     <t>Project ID</t>
   </si>
   <si>
     <t>don’t modify these three colomn, they are for the drop down lists</t>
   </si>
   <si>
-    <t>don’t know what project</t>
-  </si>
-  <si>
     <t>Showcase space needed =&gt;</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>g</t>
-  </si>
-  <si>
-    <t>h</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>i</t>
-  </si>
-  <si>
-    <t>j</t>
-  </si>
-  <si>
-    <t>k</t>
-  </si>
-  <si>
-    <t>l</t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>n</t>
-  </si>
-  <si>
-    <t>o</t>
-  </si>
-  <si>
-    <t>p</t>
-  </si>
-  <si>
-    <t>q</t>
-  </si>
-  <si>
-    <t>r</t>
+    <t>Proj 16 - Craft Matrix_Human Powered Land Vehicles</t>
+  </si>
+  <si>
+    <t>Proj S11 - NHB_Spatial Autonomy</t>
+  </si>
+  <si>
+    <t>Proj S16 - STEE_Floatsam</t>
+  </si>
+  <si>
+    <t>Proj 12 - BCA_3D printed components</t>
+  </si>
+  <si>
+    <t>Proj 54 - Samsung_REFARDEN</t>
+  </si>
+  <si>
+    <t>Proj S17 - Sunflower_Nursery</t>
+  </si>
+  <si>
+    <t>Proj S02 - Bandwagon_Music Royalty</t>
+  </si>
+  <si>
+    <t>Proj 30 - MND_Minimizing Bird Nuisance</t>
+  </si>
+  <si>
+    <t>Proj 09 - BCA_Mixed Mode Ventilation</t>
+  </si>
+  <si>
+    <t>Proj 34 - My Nonna_Project CARE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proj S07 - Hope_Legged Robotic </t>
+  </si>
+  <si>
+    <t>Proj 69 - WHC_Public Wheelchair Management</t>
+  </si>
+  <si>
+    <t>Proj 55 - Samsung_Shooshoe</t>
+  </si>
+  <si>
+    <t>Proj S03 - Certis_Security  Robot</t>
+  </si>
+  <si>
+    <t>Proj S15 - Flexi Systems_Recycling</t>
+  </si>
+  <si>
+    <t>Proj S08-HOPE_Kommunal</t>
+  </si>
+  <si>
+    <t>Proj S04-DSO_Counter-Terrorist Bot</t>
+  </si>
+  <si>
+    <t>Proj E03 - BiFrost</t>
+  </si>
+  <si>
+    <t>Proj S13 - Panasonic_P-Cube</t>
+  </si>
+  <si>
+    <t>Proj 35 - NNI Chinese Predictive</t>
+  </si>
+  <si>
+    <t>Proj 24 - Infineon_Chatbot Packing Assistant</t>
+  </si>
+  <si>
+    <t>Proj 11 - BCA_Reengineering Road Construction</t>
+  </si>
+  <si>
+    <t>Proj 59 - SERI_Predictive Data Analytics</t>
+  </si>
+  <si>
+    <t>Proj 01 - Accenture_Digital Consultant</t>
+  </si>
+  <si>
+    <t>Proj E01 - Myx Brewery</t>
+  </si>
+  <si>
+    <t>Proj 07 - Bev Eat_F&amp;B ordering &amp; donated meal claims</t>
+  </si>
+  <si>
+    <t>Proj 32 - MSF_Refurbishment of ROMM</t>
+  </si>
+  <si>
+    <t>Proj S09 - Jublia_Sparse Datasets</t>
+  </si>
+  <si>
+    <t>Proj 43-PA_Future of Service Delivery</t>
+  </si>
+  <si>
+    <t>Proj 17 - DBS_Future of Banking Branch Design</t>
+  </si>
+  <si>
+    <t>library</t>
+  </si>
+  <si>
+    <t>Proj 45 - PICO_Musical Engineering Installation</t>
+  </si>
+  <si>
+    <t>Proj 50 - Queensway Sec Sch_Design for Reading</t>
+  </si>
+  <si>
+    <t>Proj 10 - BCA_Net Zero Energy Buildings</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Proj 13 - CGH_Redesign Ward 14</t>
+  </si>
+  <si>
+    <t>Proj 36 - NNI_Exoskeleton</t>
+  </si>
+  <si>
+    <t>Proj S01 - Arup_Empowering spaces</t>
+  </si>
+  <si>
+    <t>Proj 31 - MSF_Immersive Rehabilitative Learning</t>
+  </si>
+  <si>
+    <t>Proj 46 - PICO_Creative Data Visualisation</t>
+  </si>
+  <si>
+    <t>Proj S18-V-key_Blockchain</t>
+  </si>
+  <si>
+    <t>Proj 44 - Philips_Analytics for Signify Managed Data</t>
+  </si>
+  <si>
+    <t>Proj 21 - FinC_MoneyGYM Mobile App</t>
+  </si>
+  <si>
+    <t>Proj P47 - P&amp;G_Combing</t>
+  </si>
+  <si>
+    <t>Proj E02 - Valte</t>
+  </si>
+  <si>
+    <t>Proj 15 - Citibank_Redesign Commercial Banking</t>
+  </si>
+  <si>
+    <t>Proj E05 - IOT</t>
   </si>
 </sst>
 </file>
@@ -483,27 +561,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE1AA138-B054-4B8D-B872-011631B65C70}">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44:C46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" customWidth="1"/>
-    <col min="5" max="5" width="24.42578125" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" customWidth="1"/>
+    <col min="2" max="2" width="46.21875" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" customWidth="1"/>
+    <col min="5" max="5" width="24.44140625" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" customWidth="1"/>
+    <col min="8" max="8" width="10.88671875" customWidth="1"/>
     <col min="11" max="11" width="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -515,7 +593,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -527,17 +605,17 @@
         <v>5</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1">
         <v>4.2361111111111106E-2</v>
@@ -558,12 +636,12 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1">
         <v>4.2361111111111106E-2</v>
@@ -587,7 +665,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -616,7 +694,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -645,7 +723,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -674,12 +752,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C7" s="1">
         <v>4.2361111111111099E-2</v>
@@ -700,12 +778,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C8" s="1">
         <v>4.2361111111111099E-2</v>
@@ -726,12 +804,12 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C9" s="1">
         <v>4.2361111111111099E-2</v>
@@ -752,12 +830,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C10" s="1">
         <v>4.2361111111111099E-2</v>
@@ -778,12 +856,12 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C11" s="1">
         <v>4.2361111111111099E-2</v>
@@ -804,7 +882,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -830,7 +908,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -856,7 +934,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -882,7 +960,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -908,7 +986,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -934,7 +1012,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -960,7 +1038,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -986,7 +1064,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1012,7 +1090,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1038,7 +1116,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1064,9 +1142,503 @@
         <v>10</v>
       </c>
     </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="1">
+        <v>4.2361111111111099E-2</v>
+      </c>
+      <c r="D22" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22">
+        <v>2</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="1">
+        <v>4.2361111111111099E-2</v>
+      </c>
+      <c r="D23" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23">
+        <v>3</v>
+      </c>
+      <c r="G23">
+        <v>2</v>
+      </c>
+      <c r="H23">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="1">
+        <v>4.2361111111111099E-2</v>
+      </c>
+      <c r="D24" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24">
+        <v>2</v>
+      </c>
+      <c r="G24">
+        <v>2</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="1">
+        <v>4.2361111111111099E-2</v>
+      </c>
+      <c r="D25" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25">
+        <v>2</v>
+      </c>
+      <c r="G25">
+        <v>2</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" s="1">
+        <v>4.2361111111111099E-2</v>
+      </c>
+      <c r="D26" t="s">
+        <v>6</v>
+      </c>
+      <c r="F26">
+        <v>2</v>
+      </c>
+      <c r="G26">
+        <v>2</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="1">
+        <v>4.2361111111111099E-2</v>
+      </c>
+      <c r="D27" t="s">
+        <v>8</v>
+      </c>
+      <c r="F27">
+        <v>2</v>
+      </c>
+      <c r="G27">
+        <v>2</v>
+      </c>
+      <c r="H27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" s="1">
+        <v>4.2361111111111099E-2</v>
+      </c>
+      <c r="D28" t="s">
+        <v>6</v>
+      </c>
+      <c r="F28">
+        <v>2</v>
+      </c>
+      <c r="G28">
+        <v>2</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" s="1">
+        <v>4.2361111111111099E-2</v>
+      </c>
+      <c r="D29" t="s">
+        <v>8</v>
+      </c>
+      <c r="F29">
+        <v>5</v>
+      </c>
+      <c r="G29">
+        <v>4</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30" s="1">
+        <v>4.2361111111111099E-2</v>
+      </c>
+      <c r="D30" t="s">
+        <v>6</v>
+      </c>
+      <c r="F30">
+        <v>3</v>
+      </c>
+      <c r="G30">
+        <v>2</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" s="1">
+        <v>4.2361111111111099E-2</v>
+      </c>
+      <c r="D31" t="s">
+        <v>8</v>
+      </c>
+      <c r="F31">
+        <v>3.5</v>
+      </c>
+      <c r="G31">
+        <v>3.5</v>
+      </c>
+      <c r="H31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>44</v>
+      </c>
+      <c r="C32" s="1">
+        <v>4.2361111111111099E-2</v>
+      </c>
+      <c r="D32" t="s">
+        <v>6</v>
+      </c>
+      <c r="F32">
+        <v>4</v>
+      </c>
+      <c r="G32">
+        <v>4</v>
+      </c>
+      <c r="H32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" s="1">
+        <v>4.2361111111111099E-2</v>
+      </c>
+      <c r="D33" t="s">
+        <v>8</v>
+      </c>
+      <c r="F33">
+        <v>5</v>
+      </c>
+      <c r="G33">
+        <v>4</v>
+      </c>
+      <c r="H33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>46</v>
+      </c>
+      <c r="C34" s="1">
+        <v>4.2361111111111099E-2</v>
+      </c>
+      <c r="D34" t="s">
+        <v>6</v>
+      </c>
+      <c r="F34">
+        <v>3.5</v>
+      </c>
+      <c r="G34">
+        <v>3</v>
+      </c>
+      <c r="H34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>47</v>
+      </c>
+      <c r="C35" s="1">
+        <v>4.2361111111111099E-2</v>
+      </c>
+      <c r="D35" t="s">
+        <v>8</v>
+      </c>
+      <c r="F35">
+        <v>5</v>
+      </c>
+      <c r="G35">
+        <v>5</v>
+      </c>
+      <c r="H35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>48</v>
+      </c>
+      <c r="C36" s="1">
+        <v>4.2361111111111099E-2</v>
+      </c>
+      <c r="D36" t="s">
+        <v>6</v>
+      </c>
+      <c r="F36">
+        <v>3</v>
+      </c>
+      <c r="G36">
+        <v>3</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>49</v>
+      </c>
+      <c r="C37" s="1">
+        <v>4.2361111111111099E-2</v>
+      </c>
+      <c r="D37" t="s">
+        <v>8</v>
+      </c>
+      <c r="F37">
+        <v>2</v>
+      </c>
+      <c r="G37">
+        <v>2</v>
+      </c>
+      <c r="H37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>50</v>
+      </c>
+      <c r="C38" s="1">
+        <v>4.2361111111111099E-2</v>
+      </c>
+      <c r="D38" t="s">
+        <v>6</v>
+      </c>
+      <c r="F38" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>51</v>
+      </c>
+      <c r="C39" s="1">
+        <v>4.2361111111111099E-2</v>
+      </c>
+      <c r="D39" t="s">
+        <v>8</v>
+      </c>
+      <c r="F39">
+        <v>2</v>
+      </c>
+      <c r="G39">
+        <v>2</v>
+      </c>
+      <c r="H39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>52</v>
+      </c>
+      <c r="C40" s="1">
+        <v>4.2361111111111099E-2</v>
+      </c>
+      <c r="D40" t="s">
+        <v>6</v>
+      </c>
+      <c r="F40">
+        <v>2</v>
+      </c>
+      <c r="G40">
+        <v>2</v>
+      </c>
+      <c r="H40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>53</v>
+      </c>
+      <c r="C41" s="1">
+        <v>4.2361111111111099E-2</v>
+      </c>
+      <c r="D41" t="s">
+        <v>8</v>
+      </c>
+      <c r="F41">
+        <v>2</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
+      <c r="H41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>54</v>
+      </c>
+      <c r="C42" s="1">
+        <v>4.2361111111111099E-2</v>
+      </c>
+      <c r="D42" t="s">
+        <v>8</v>
+      </c>
+      <c r="F42">
+        <v>2.5</v>
+      </c>
+      <c r="G42">
+        <v>2.5</v>
+      </c>
+      <c r="H42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>55</v>
+      </c>
+      <c r="C43" s="1">
+        <v>4.2361111111111099E-2</v>
+      </c>
+      <c r="D43" t="s">
+        <v>6</v>
+      </c>
+      <c r="F43">
+        <v>3</v>
+      </c>
+      <c r="G43">
+        <v>2</v>
+      </c>
+      <c r="H43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
+        <v>56</v>
+      </c>
+      <c r="C44" s="1">
+        <v>4.2361111111111099E-2</v>
+      </c>
+      <c r="D44" t="s">
+        <v>8</v>
+      </c>
+      <c r="F44">
+        <v>2.5</v>
+      </c>
+      <c r="G44">
+        <v>2.5</v>
+      </c>
+      <c r="H44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>57</v>
+      </c>
+      <c r="C45" s="1">
+        <v>4.2361111111111099E-2</v>
+      </c>
+      <c r="D45" t="s">
+        <v>6</v>
+      </c>
+      <c r="F45">
+        <v>2</v>
+      </c>
+      <c r="G45">
+        <v>2</v>
+      </c>
+      <c r="H45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
+        <v>58</v>
+      </c>
+      <c r="C46" s="1">
+        <v>4.2361111111111099E-2</v>
+      </c>
+      <c r="D46" t="s">
+        <v>8</v>
+      </c>
+      <c r="F46">
+        <v>2</v>
+      </c>
+      <c r="G46">
+        <v>2</v>
+      </c>
+      <c r="H46">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:E3 E5:E22 D4:D22" xr:uid="{2AA1476B-CB50-4057-B8B9-3F1890D45CA0}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:E3 E5:E22 D4:D46" xr:uid="{2AA1476B-CB50-4057-B8B9-3F1890D45CA0}">
       <formula1>$K$3:$K$6</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:H32" xr:uid="{A358D48E-311D-4BC6-8032-2DBDB58F8DD0}">

</xml_diff>